<commit_message>
correction test assets: removed trailing space from _customVoc sheet
</commit_message>
<xml_diff>
--- a/tests/assets/data2-custom-and-missing-voc.xlsx
+++ b/tests/assets/data2-custom-and-missing-voc.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A437049-1B1E-4BEC-8D2E-0613F14B4F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16597CC-9AC8-43D2-B910-9C1C49BD9267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreatiefWerk" sheetId="1" r:id="rId1"/>
     <sheet name="Licentie" sheetId="2" r:id="rId2"/>
     <sheet name="Agent" sheetId="4" r:id="rId3"/>
     <sheet name="Boek" sheetId="5" r:id="rId4"/>
-    <sheet name="_customVoc " sheetId="6" r:id="rId5"/>
+    <sheet name="_customVoc" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -1129,7 +1129,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B13" sqref="B13"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>